<commit_message>
A few details again
</commit_message>
<xml_diff>
--- a/output/compo scats/summary_scats_compo.xlsx
+++ b/output/compo scats/summary_scats_compo.xlsx
@@ -23,25 +23,25 @@
     <t xml:space="preserve">n</t>
   </si>
   <si>
-    <t xml:space="preserve">conc_mg_g_dw_min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc_mg_g_dw_low_quant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc_mg_g_dw_mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc_mg_g_dw_high_quant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc_mg_g_dw_max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc_mg_g_dw_sd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc_mg_g_dw_cv</t>
+    <t xml:space="preserve">conc_mg_kg_dw_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc_mg_kg_dw_low_quant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc_mg_kg_dw_mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc_mg_kg_dw_high_quant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc_mg_kg_dw_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc_mg_kg_dw_sd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc_mg_kg_dw_cv</t>
   </si>
   <si>
     <t xml:space="preserve">Cap Noir</t>

</xml_diff>